<commit_message>
v1.03 - IK working
</commit_message>
<xml_diff>
--- a/Inverse Kinematics.xlsx
+++ b/Inverse Kinematics.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="24">
   <si>
     <t>http://www.oliverjenkins.com/blog/2012/9/inverse-kinematics-and-robot-arms</t>
   </si>
@@ -194,18 +194,6 @@
     <t>Z should always be on table. Bottom of robot arm is 102mm (4") below θ1 pivot point</t>
   </si>
   <si>
-    <t xml:space="preserve">The problem is for my robotic arm, if θ1 changes, θ2 will change also.  In the above sketch, they are independent.  </t>
-  </si>
-  <si>
-    <t>The above sketch would be more appropriate is the servor for L2 was mounted at the L1-L2 joint</t>
-  </si>
-  <si>
-    <t>Up/Down</t>
-  </si>
-  <si>
-    <t>Fwd/Back</t>
-  </si>
-  <si>
     <t>Y Distance</t>
   </si>
   <si>
@@ -220,6 +208,24 @@
   </si>
   <si>
     <t>http://www.learnaboutrobots.com/inverseKinematics.htm</t>
+  </si>
+  <si>
+    <t>https://www.circuitsathome.com/mcu/robotic-arm-inverse-kinematics-on-arduino</t>
+  </si>
+  <si>
+    <t>bicep</t>
+  </si>
+  <si>
+    <t>forearm</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Github IK Discussion</t>
+  </si>
+  <si>
+    <t>Chart Data</t>
   </si>
 </sst>
 </file>
@@ -227,7 +233,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="7" x14ac:knownFonts="1">
     <font>
@@ -311,13 +317,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -327,6 +333,15 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -356,11 +371,138 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
       <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Inverese Kinematics Calc'!$K$38</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Z</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Inverese Kinematics Calc'!$J$39:$J$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.424543253295901</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>160</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Inverese Kinematics Calc'!$K$39:$K$41</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>135.95146158945312</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="97796864"/>
+        <c:axId val="97795072"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="97796864"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="300"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="97795072"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="97795072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="160"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="97796864"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -375,7 +517,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Fwd/Back</c:v>
+                  <c:v>bicep</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -494,11 +636,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="96070272"/>
-        <c:axId val="96034176"/>
+        <c:axId val="101995648"/>
+        <c:axId val="101997568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="96070272"/>
+        <c:axId val="101995648"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="550"/>
@@ -517,24 +659,23 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Up / Down</a:t>
+                  <a:t>Forearm</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96034176"/>
+        <c:crossAx val="101997568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="96034176"/>
+        <c:axId val="101997568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="300"/>
@@ -554,19 +695,18 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-US"/>
-                  <a:t>Fwd/Back</a:t>
+                  <a:t>Bicep</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="96070272"/>
+        <c:crossAx val="101995648"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -589,13 +729,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -638,6 +778,36 @@
         </a:extLst>
       </xdr:spPr>
     </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>409575</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>123824</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -965,10 +1135,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:K42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -980,69 +1150,53 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
-    </row>
-    <row r="5" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A26" s="2" t="s">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B27" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C27" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D27" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="2" t="s">
+      <c r="E27" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="F27" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G26" s="2" t="s">
+      <c r="G27" s="2" t="s">
         <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A27" s="3">
-        <v>9</v>
-      </c>
-      <c r="B27" s="3">
-        <v>7</v>
-      </c>
-      <c r="C27" s="3">
-        <v>7</v>
-      </c>
-      <c r="D27" s="3">
-        <v>9</v>
-      </c>
-      <c r="E27" s="3">
-        <f>SQRT(C27^2+ D27^2)</f>
-        <v>11.401754250991379</v>
-      </c>
-      <c r="F27" s="3">
-        <f>DEGREES(ATAN(D27/C27)+ ACOS((A27^2 - B27^2 + C27^2 + D27^2) / (2 * A27 * E27)))</f>
-        <v>90</v>
-      </c>
-      <c r="G27" s="3">
-        <f>DEGREES(ACOS((E27^2 - A27^2 - B27^2) / (2*A27*B27)))</f>
-        <v>90</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1053,22 +1207,22 @@
         <v>7</v>
       </c>
       <c r="C28" s="3">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D28" s="3">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E28" s="3">
         <f>SQRT(C28^2+ D28^2)</f>
-        <v>16</v>
+        <v>11.401754250991379</v>
       </c>
       <c r="F28" s="3">
         <f>DEGREES(ATAN(D28/C28)+ ACOS((A28^2 - B28^2 + C28^2 + D28^2) / (2 * A28 * E28)))</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="G28" s="3">
         <f>DEGREES(ACOS((E28^2 - A28^2 - B28^2) / (2*A28*B28)))</f>
-        <v>0</v>
+        <v>90</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1078,117 +1232,116 @@
       <c r="B29" s="3">
         <v>7</v>
       </c>
-      <c r="C29">
-        <v>11.313708399999999</v>
-      </c>
-      <c r="D29">
-        <f>C29</f>
-        <v>11.313708399999999</v>
+      <c r="C29" s="3">
+        <v>16</v>
+      </c>
+      <c r="D29" s="3">
+        <v>0</v>
       </c>
       <c r="E29" s="3">
         <f>SQRT(C29^2+ D29^2)</f>
-        <v>15.999999860014409</v>
+        <v>16</v>
       </c>
       <c r="F29" s="3">
         <f>DEGREES(ATAN(D29/C29)+ ACOS((A29^2 - B29^2 + C29^2 + D29^2) / (2 * A29 * E29)))</f>
-        <v>45.006684163672624</v>
+        <v>0</v>
       </c>
       <c r="G29" s="3">
         <f>DEGREES(ACOS((E29^2 - A29^2 - B29^2) / (2*A29*B29)))</f>
-        <v>1.5278088269047689E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="3">
-        <f>140/25.4</f>
-        <v>5.5118110236220472</v>
+        <v>9</v>
       </c>
       <c r="B30" s="3">
-        <f>153/25.4</f>
-        <v>6.0236220472440944</v>
-      </c>
-      <c r="C30" s="3">
-        <v>8</v>
-      </c>
-      <c r="D30" s="3">
-        <v>1</v>
+        <v>7</v>
+      </c>
+      <c r="C30">
+        <v>11.313708399999999</v>
+      </c>
+      <c r="D30">
+        <f>C30</f>
+        <v>11.313708399999999</v>
       </c>
       <c r="E30" s="3">
         <f>SQRT(C30^2+ D30^2)</f>
-        <v>8.0622577482985491</v>
+        <v>15.999999860014409</v>
       </c>
       <c r="F30" s="3">
         <f>DEGREES(ATAN(D30/C30)+ ACOS((A30^2 - B30^2 + C30^2 + D30^2) / (2 * A30 * E30)))</f>
-        <v>55.447891114097978</v>
+        <v>45.006684163672624</v>
       </c>
       <c r="G30" s="3">
         <f>DEGREES(ACOS((E30^2 - A30^2 - B30^2) / (2*A30*B30)))</f>
-        <v>91.436022162277041</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+        <v>1.5278088269047689E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="3">
+        <v>140</v>
+      </c>
+      <c r="B31" s="3">
+        <v>153</v>
+      </c>
+      <c r="C31" s="3">
+        <v>242</v>
+      </c>
+      <c r="D31" s="3">
+        <v>150</v>
+      </c>
+      <c r="E31" s="3">
+        <f>SQRT(C31^2+ D31^2)</f>
+        <v>284.7174037532655</v>
+      </c>
+      <c r="F31" s="3">
+        <f>DEGREES(ATAN(D31/C31)+ ACOS((A31^2 - B31^2 + C31^2 + D31^2) / (2 * A31 * E31)))</f>
+        <v>46.079787548492433</v>
+      </c>
+      <c r="G31" s="3">
+        <f>DEGREES(ACOS((E31^2 - A31^2 - B31^2) / (2*A31*B31)))</f>
+        <v>27.338939098316182</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="2" t="s">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="B37" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C36" s="2" t="s">
+      <c r="C37" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="2" t="s">
+      <c r="D37" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E36" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F36" s="2" t="s">
+      <c r="F37" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G36" s="2" t="s">
+      <c r="G37" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="3">
-        <f>140/25.4</f>
-        <v>5.5118110236220472</v>
-      </c>
-      <c r="B37" s="3">
-        <f>153/25.4</f>
-        <v>6.0236220472440944</v>
-      </c>
-      <c r="C37" s="3">
-        <v>8</v>
-      </c>
-      <c r="D37" s="3">
-        <f>-102/25.4 + 1.5</f>
-        <v>-2.515748031496063</v>
-      </c>
-      <c r="E37" s="3">
-        <f>SQRT(C37^2+ D37^2)</f>
-        <v>8.3862380217816561</v>
-      </c>
-      <c r="F37" s="3">
-        <f>DEGREES(ATAN(D37/C37)+ ACOS((A37^2 - B37^2 + C37^2 + D37^2) / (2 * A37 * E37)))</f>
-        <v>28.365407207543488</v>
-      </c>
-      <c r="G37" s="3">
-        <f>DEGREES(ACOS((E37^2 - A37^2 - B37^2) / (2*A37*B37)))</f>
-        <v>86.836090559429792</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J37" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="K37" s="9"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="3">
         <v>140</v>
       </c>
@@ -1196,41 +1349,73 @@
         <v>153</v>
       </c>
       <c r="C38" s="3">
-        <v>200</v>
+        <v>160</v>
       </c>
       <c r="D38" s="3">
-        <v>-64</v>
+        <v>50</v>
       </c>
       <c r="E38" s="3">
         <f>SQRT(C38^2+ D38^2)</f>
-        <v>209.99047597450701</v>
+        <v>167.6305461424021</v>
       </c>
       <c r="F38" s="3">
         <f>DEGREES(ATAN(D38/C38)+ ACOS((A38^2 - B38^2 + C38^2 + D38^2) / (2 * A38 * E38)))</f>
-        <v>29.005238249737474</v>
+        <v>76.187416394759182</v>
       </c>
       <c r="G38" s="3">
         <f>DEGREES(ACOS((E38^2 - A38^2 - B38^2) / (2*A38*B38)))</f>
-        <v>88.546050487675103</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>14</v>
-      </c>
+        <v>110.36600497260855</v>
+      </c>
+      <c r="J38" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K38" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J39" s="10">
+        <v>0</v>
+      </c>
+      <c r="K39" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J40" s="10">
+        <f>COS(RADIANS(F38)) * A38</f>
+        <v>33.424543253295901</v>
+      </c>
+      <c r="K40" s="10">
+        <f>SIN(RADIANS(F38)) * A38</f>
+        <v>135.95146158945312</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J41" s="10">
+        <f>C38</f>
+        <v>160</v>
+      </c>
+      <c r="K41" s="10">
+        <f>D38</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="J42" s="6"/>
+      <c r="K42" s="6"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="J37:K37"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="A33" r:id="rId1"/>
+    <hyperlink ref="A34" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2" location="issuecomment-138402648"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
 
@@ -1239,7 +1424,7 @@
   <dimension ref="B1:J12"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1253,19 +1438,19 @@
   <sheetData>
     <row r="1" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="B1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E1" s="7" t="s">
-        <v>19</v>
-      </c>
       <c r="F1" s="7" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="G1" s="7"/>
     </row>
@@ -1309,7 +1494,7 @@
       </c>
       <c r="G3" s="4"/>
       <c r="J3" s="8" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
@@ -1431,6 +1616,9 @@
         <v>-11.857945000000427</v>
       </c>
       <c r="G9" s="4"/>
+      <c r="H9" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="10" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B10" s="6">

</xml_diff>